<commit_message>
Generate task stamps from excel
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinhhoang/Documents/pay-me/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EB73EC-81B4-483F-8A0D-6BF65F67A7B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89EE156-98F4-674F-8368-1BAE2F762A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10300" yWindow="1320" windowWidth="20940" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="Subs" sheetId="2" r:id="rId2"/>
+    <sheet name="Subsubs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,69 +27,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SELECTED</t>
-  </si>
-  <si>
-    <t>REWARD</t>
-  </si>
-  <si>
-    <t>CNVX OPTMZ 2H</t>
-  </si>
-  <si>
-    <t>Complete Chapter 2</t>
-  </si>
-  <si>
-    <t>CNVOP</t>
-  </si>
-  <si>
-    <t>LEARN</t>
-  </si>
-  <si>
-    <t>LRN FR PRCPLE 2H</t>
-  </si>
-  <si>
-    <t>Recite Chapter 2 and continue Chapter 3</t>
-  </si>
-  <si>
-    <t>PROBT</t>
-  </si>
-  <si>
-    <t>PROBA THRY 2H</t>
-  </si>
-  <si>
-    <t>Next 7 pages</t>
-  </si>
-  <si>
-    <t>RSRC1</t>
-  </si>
-  <si>
-    <t>RSC PAPER 2H</t>
-  </si>
-  <si>
-    <t>Read some papers in the field</t>
-  </si>
-  <si>
-    <t>RSRC2</t>
-  </si>
-  <si>
-    <t>RSC CODE 2H</t>
-  </si>
-  <si>
-    <t>Perform some coding of the idea</t>
-  </si>
-  <si>
-    <t>EXPIRED</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+  <si>
+    <t>DAILY</t>
+  </si>
+  <si>
+    <t>Daily Time Allocation</t>
+  </si>
+  <si>
+    <t>Daily time stamp for …</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>tname</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>unselected</t>
+  </si>
+  <si>
+    <t>expired</t>
+  </si>
+  <si>
+    <t>sname</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>Proba Thry</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Thm 2.13.1</t>
+  </si>
+  <si>
+    <t>Thm 2.13.2</t>
+  </si>
+  <si>
+    <t>3 days</t>
   </si>
 </sst>
 </file>
@@ -406,139 +396,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E857AE8B-8A67-6744-8C9A-D8523DC2B8EF}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data format fixes for CSV
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinhhoang/Documents/pay-me/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89EE156-98F4-674F-8368-1BAE2F762A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A17CA9C-A375-C843-AF41-E41655F6AECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10300" yWindow="1320" windowWidth="20940" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>DAILY</t>
   </si>
@@ -396,20 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -423,10 +421,13 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -439,7 +440,10 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parsing countUp tasks in easy_csv
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5BE17D-BB60-4B0E-9990-81094D69F302}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515BC715-4734-4262-917D-ED48AD281C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>DAILY</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Daily time stamp for 20/10/2021</t>
+  </si>
+  <si>
+    <t>countUp</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -480,15 +483,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -504,8 +507,11 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -538,8 +544,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -556,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -574,7 +583,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E1:E1048576 F1 F3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
countUp tasks should not have time field
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515BC715-4734-4262-917D-ED48AD281C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DF560B-8D5B-48EA-BF8D-94599D396897}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>DAILY</t>
   </si>
@@ -89,10 +89,19 @@
     <t>Lm-Thm 3.7-8</t>
   </si>
   <si>
-    <t>Daily time stamp for 20/10/2021</t>
-  </si>
-  <si>
     <t>countUp</t>
+  </si>
+  <si>
+    <t>Cours S5</t>
+  </si>
+  <si>
+    <t>TP S5</t>
+  </si>
+  <si>
+    <t>Daily time stamp for 24/10/2021</t>
+  </si>
+  <si>
+    <t>Distr convolution</t>
   </si>
 </sst>
 </file>
@@ -425,7 +434,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -485,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -573,13 +582,13 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -594,9 +603,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E857AE8B-8A67-6744-8C9A-D8523DC2B8EF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -635,13 +644,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -649,10 +658,43 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync countUp and time status
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DF560B-8D5B-48EA-BF8D-94599D396897}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E860EF-6E8E-4E25-9B86-F7CD095563FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,9 +552,6 @@
       </c>
       <c r="E3">
         <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -605,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E857AE8B-8A67-6744-8C9A-D8523DC2B8EF}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>

<commit_message>
Reset habits to today
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -8,26 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E860EF-6E8E-4E25-9B86-F7CD095563FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4BDED0-0D3A-4050-82CB-BDFCE6308F7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Subs" sheetId="2" r:id="rId2"/>
     <sheet name="Subsubs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>DAILY</t>
   </si>
@@ -68,40 +77,22 @@
     <t>name</t>
   </si>
   <si>
+    <t>countUp</t>
+  </si>
+  <si>
+    <t>Info Thry</t>
+  </si>
+  <si>
+    <t>Cpr Sens</t>
+  </si>
+  <si>
     <t>3 days</t>
   </si>
   <si>
-    <t>Quick Det</t>
-  </si>
-  <si>
-    <t>Teaching</t>
-  </si>
-  <si>
-    <t>Pg 103-105</t>
-  </si>
-  <si>
-    <t>Mthd PCA-TD</t>
-  </si>
-  <si>
-    <t>LN Thm 3.5</t>
-  </si>
-  <si>
-    <t>Lm-Thm 3.7-8</t>
-  </si>
-  <si>
-    <t>countUp</t>
-  </si>
-  <si>
-    <t>Cours S5</t>
-  </si>
-  <si>
-    <t>TP S5</t>
-  </si>
-  <si>
-    <t>Daily time stamp for 24/10/2021</t>
-  </si>
-  <si>
-    <t>Distr convolution</t>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Daily time stamp for 11/12/2021</t>
   </si>
 </sst>
 </file>
@@ -144,7 +135,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -433,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -472,7 +493,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -481,7 +502,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -492,15 +513,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -517,10 +538,13 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -536,33 +560,41 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="str">
+        <f>IF(C2&gt;0,"TRUE",IF(AND(C2=0,E2=0,F2&lt;&gt;1),"INVALID",IF(F2=1,"TRUE","FALSE")))</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(C3&gt;0,"TRUE",IF(AND(C3=0,E3=0,F3&lt;&gt;1),"INVALID",IF(F3=1,"TRUE","FALSE")))</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -570,8 +602,15 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(C4&gt;0,"TRUE",IF(AND(C4=0,E4=0,F4&lt;&gt;1),"INVALID",IF(F4=1,"TRUE","FALSE")))</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -579,19 +618,34 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <f>IF(C5&gt;0,"TRUE",IF(AND(C5=0,E5=0,F5&lt;&gt;1),"INVALID",IF(F5=1,"TRUE","FALSE")))</f>
+        <v>FALSE</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576 F1 F3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="E1:E1048576 F1:G1 F4:F5 F2">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"TRUE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"""TRUE"""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -600,11 +654,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E857AE8B-8A67-6744-8C9A-D8523DC2B8EF}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="165" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -617,84 +671,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>2.5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allow transfer expired date from XLS and fix the relative path
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinhhoang/Documents/pay-me/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4803846A-39FD-45BA-BBBF-0BF9D2F0F407}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9BED2A-91AE-C340-A08A-16DCE85420B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1640" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -98,13 +98,13 @@
     <t>Wavelet</t>
   </si>
   <si>
-    <t>R2-3.1</t>
-  </si>
-  <si>
-    <t>Plan for 31/01/2022</t>
-  </si>
-  <si>
-    <t>D-Slides</t>
+    <t>Plan for 02/02/2022</t>
+  </si>
+  <si>
+    <t>R-4.1,2,4</t>
+  </si>
+  <si>
+    <t>D-Wavelet</t>
   </si>
 </sst>
 </file>
@@ -470,14 +470,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -528,12 +528,12 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -556,7 +556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -577,7 +577,7 @@
         <v>FALSE</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -598,7 +598,7 @@
         <v>FALSE</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -622,7 +622,7 @@
         <v>TRUE</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -643,7 +643,7 @@
         <v>TRUE</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -691,9 +691,9 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -704,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -715,18 +715,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -734,7 +734,7 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving payrate to an extern variable
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinhhoang/Documents/pay-me/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9BED2A-91AE-C340-A08A-16DCE85420B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321437E6-6DD1-4C49-A37C-21C30FB452C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1640" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>DAILY</t>
   </si>
@@ -92,29 +92,51 @@
     <t>Func Anal</t>
   </si>
   <si>
-    <t>R-63,64,65</t>
-  </si>
-  <si>
     <t>Wavelet</t>
   </si>
   <si>
-    <t>Plan for 02/02/2022</t>
-  </si>
-  <si>
-    <t>R-4.1,2,4</t>
-  </si>
-  <si>
-    <t>D-Wavelet</t>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Comp Sens</t>
+  </si>
+  <si>
+    <t>Diff Geom</t>
+  </si>
+  <si>
+    <t>Har Anal</t>
+  </si>
+  <si>
+    <t>R-4</t>
+  </si>
+  <si>
+    <t>R-5</t>
+  </si>
+  <si>
+    <t>D-Segment</t>
+  </si>
+  <si>
+    <t>Plan for 05/03/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,14 +162,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -467,17 +530,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="35.6328125" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -497,7 +560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -505,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -525,15 +588,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -556,7 +619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -573,11 +636,11 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(C2&gt;0,"TRUE",IF(AND(C2=0,E2=0,F2&lt;&gt;1),"INVALID",IF(F2=1,"TRUE","FALSE")))</f>
+        <f>IF(E2=1,"FALSE",IF(OR(AND((C2&gt;0),(F2="")),AND(F2=1, C2=0)),"TRUE","FALSE"))</f>
         <v>FALSE</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -594,19 +657,19 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(C3&gt;0,"TRUE",IF(AND(C3=0,E3=0,F3&lt;&gt;1),"INVALID",IF(F3=1,"TRUE","FALSE")))</f>
+        <f t="shared" ref="G3:G11" si="0">IF(E3=1,"FALSE",IF(OR(AND((C3&gt;0),(F3="")),AND(F3=1, C3=0)),"TRUE","FALSE"))</f>
         <v>FALSE</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -614,44 +677,41 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
       <c r="G4" t="str">
-        <f>IF(C4&gt;0,"TRUE",IF(AND(C4=0,E4=0,F4&lt;&gt;1),"INVALID",IF(F4=1,"TRUE","FALSE")))</f>
+        <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="str">
-        <f>IF(C5&gt;0,"TRUE",IF(AND(C5=0,E5=0,F5&lt;&gt;1),"INVALID",IF(F5=1,"TRUE","FALSE")))</f>
-        <v>TRUE</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+        <f t="shared" si="0"/>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -660,25 +720,148 @@
         <v>0</v>
       </c>
       <c r="G6" t="str">
-        <f>IF(C6&gt;0,"TRUE",IF(AND(C6=0,E6=0,F6&lt;&gt;1),"INVALID",IF(F6=1,"TRUE","FALSE")))</f>
+        <f t="shared" si="0"/>
         <v>TRUE</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>FALSE</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576 F1:G1 F2:F5">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="F1:G1 F2:F5 E1:E1048576 F7">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"""TRUE"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -691,9 +874,9 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -704,37 +887,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a totalReward field
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf67027\Documents\PayMe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinhhoang/Documents/pay-me/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321437E6-6DD1-4C49-A37C-21C30FB452C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FE7382-62CE-6E40-9F55-24F55BD4E6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3140" yWindow="2040" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>DAILY</t>
   </si>
@@ -101,32 +101,38 @@
     <t>Groups</t>
   </si>
   <si>
-    <t>Comp Sens</t>
-  </si>
-  <si>
     <t>Diff Geom</t>
   </si>
   <si>
     <t>Har Anal</t>
   </si>
   <si>
-    <t>R-4</t>
-  </si>
-  <si>
-    <t>R-5</t>
-  </si>
-  <si>
-    <t>D-Segment</t>
-  </si>
-  <si>
-    <t>Plan for 05/03/2022</t>
+    <t>R-SSA1</t>
+  </si>
+  <si>
+    <t>Sps Com</t>
+  </si>
+  <si>
+    <t>R-2</t>
+  </si>
+  <si>
+    <t>W-Elad3</t>
+  </si>
+  <si>
+    <t>Plan for 27/4/2022</t>
+  </si>
+  <si>
+    <t>R-Elad3</t>
+  </si>
+  <si>
+    <t>P-Linear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,15 +174,96 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -530,17 +623,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -560,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -590,13 +683,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BB224F-5E77-174A-A6B4-EC40900F13D9}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A3" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -619,7 +712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -640,7 +733,7 @@
         <v>FALSE</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -657,37 +750,37 @@
         <v>1</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G11" si="0">IF(E3=1,"FALSE",IF(OR(AND((C3&gt;0),(F3="")),AND(F3=1, C3=0)),"TRUE","FALSE"))</f>
+        <f t="shared" ref="G3:G8" si="0">IF(E3=1,"FALSE",IF(OR(AND((C3&gt;0),(F3="")),AND(F3=1, C3=0)),"TRUE","FALSE"))</f>
         <v>FALSE</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+        <f>IF(E4=1,"FALSE",IF(OR(AND((C4&gt;0),(F4="")),AND(F4=1, C4=0)),"TRUE","FALSE"))</f>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -703,33 +796,33 @@
         <v>FALSE</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>TRUE</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -745,12 +838,12 @@
         <v>FALSE</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -766,76 +859,110 @@
         <v>FALSE</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <f>IF(E9=1,"FALSE",IF(OR(AND((C9&gt;0),(F9="")),AND(F9=1, C9=0)),"TRUE","FALSE"))</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f>IF(E10=1,"FALSE",IF(OR(AND((C10&gt;0),(F10="")),AND(F10=1, C10=0)),"TRUE","FALSE"))</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>FALSE</v>
+        <f>IF(E11=1,"FALSE",IF(OR(AND((C11&gt;0),(F11="")),AND(F11=1, C11=0)),"TRUE","FALSE"))</f>
+        <v>TRUE</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:G1 F2:F5 E1:E1048576 F7">
+  <conditionalFormatting sqref="F1:G1 F6 F9 E12:E1048576 F2:F4 E1:E10">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12:G1048576 G1:G10">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"TRUE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"""TRUE"""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C1048576 C1:C10">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F1048576 F1:F10">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E1048576 E1:E10">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:F11">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="G11">
     <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
@@ -846,7 +973,7 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -854,12 +981,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
+  <conditionalFormatting sqref="F11">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E11">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -870,13 +997,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E857AE8B-8A67-6744-8C9A-D8523DC2B8EF}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -887,37 +1016,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
+      <c r="C6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>